<commit_message>
OS, systems, and adapters parsed. Need to split Agentless entries.
</commit_message>
<xml_diff>
--- a/15C-Red-BOM-2015-10-19.xlsx
+++ b/15C-Red-BOM-2015-10-19.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbothwell/Box Sync/UX Packages/UX Package BOMs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-34460" yWindow="560" windowWidth="29500" windowHeight="20380"/>
   </bookViews>
@@ -1893,7 +1888,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2184,6 +2179,56 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2193,15 +2238,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2211,53 +2247,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="168">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2482,7 +2474,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2517,7 +2509,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2729,10 +2721,10 @@
   <dimension ref="A1:Z76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="2"/>
     <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
@@ -2761,54 +2753,54 @@
     <col min="25" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+    <row r="1" spans="1:26" ht="18">
+      <c r="A1" s="111" t="s">
         <v>403</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-    </row>
-    <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="B1" s="111"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+    </row>
+    <row r="2" spans="1:26" ht="18">
+      <c r="A2" s="111" t="s">
         <v>404</v>
       </c>
-      <c r="B2" s="135"/>
-    </row>
-    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="111"/>
+    </row>
+    <row r="4" spans="1:26" ht="15">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="131" t="s">
         <v>407</v>
       </c>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="133"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="116" t="s">
+      <c r="H4" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="118"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="133"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="116" t="s">
+      <c r="N4" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="117"/>
-      <c r="U4" s="117"/>
-      <c r="V4" s="117"/>
-      <c r="W4" s="117"/>
-      <c r="X4" s="118"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="O4" s="132"/>
+      <c r="P4" s="132"/>
+      <c r="Q4" s="132"/>
+      <c r="R4" s="132"/>
+      <c r="S4" s="132"/>
+      <c r="T4" s="132"/>
+      <c r="U4" s="132"/>
+      <c r="V4" s="132"/>
+      <c r="W4" s="132"/>
+      <c r="X4" s="133"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="B5" s="88" t="s">
         <v>51</v>
       </c>
@@ -2873,24 +2865,24 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="B6" s="89" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="114"/>
-      <c r="F6" s="115"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="113" t="s">
+      <c r="H6" s="125" t="s">
         <v>208</v>
       </c>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="115"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
       <c r="M6" s="24"/>
       <c r="N6" s="97" t="s">
         <v>9</v>
@@ -2928,7 +2920,7 @@
       <c r="Y6" s="76"/>
       <c r="Z6" s="25"/>
     </row>
-    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="28">
       <c r="B7" s="90" t="s">
         <v>238</v>
       </c>
@@ -2995,7 +2987,7 @@
       <c r="Y7" s="76"/>
       <c r="Z7" s="32"/>
     </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="28">
       <c r="B8" s="90" t="s">
         <v>302</v>
       </c>
@@ -3059,7 +3051,7 @@
       <c r="Y8" s="76"/>
       <c r="Z8" s="32"/>
     </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="28">
       <c r="B9" s="92" t="s">
         <v>232</v>
       </c>
@@ -3123,7 +3115,7 @@
       <c r="Y9" s="76"/>
       <c r="Z9" s="32"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="B10" s="90" t="s">
         <v>303</v>
       </c>
@@ -3170,7 +3162,7 @@
       <c r="Y10" s="76"/>
       <c r="Z10" s="32"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="B11" s="92" t="s">
         <v>231</v>
       </c>
@@ -3185,13 +3177,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="113" t="s">
+      <c r="H11" s="125" t="s">
         <v>209</v>
       </c>
-      <c r="I11" s="114"/>
-      <c r="J11" s="114"/>
-      <c r="K11" s="114"/>
-      <c r="L11" s="115"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="127"/>
       <c r="N11" s="64" t="s">
         <v>285</v>
       </c>
@@ -3224,7 +3216,7 @@
       <c r="Y11" s="76"/>
       <c r="Z11" s="32"/>
     </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="28">
       <c r="B12" s="90" t="s">
         <v>304</v>
       </c>
@@ -3239,7 +3231,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="120" t="s">
+      <c r="H12" s="116" t="s">
         <v>335</v>
       </c>
       <c r="I12" s="95" t="s">
@@ -3283,7 +3275,7 @@
       <c r="Y12" s="76"/>
       <c r="Z12" s="32"/>
     </row>
-    <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="28">
       <c r="B13" s="90" t="s">
         <v>233</v>
       </c>
@@ -3298,7 +3290,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="H13" s="121"/>
+      <c r="H13" s="134"/>
       <c r="I13" s="95" t="s">
         <v>185</v>
       </c>
@@ -3340,12 +3332,12 @@
       <c r="Y13" s="76"/>
       <c r="Z13" s="32"/>
     </row>
-    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="28">
       <c r="B14" s="90" t="s">
         <v>390</v>
       </c>
       <c r="C14" s="43"/>
-      <c r="H14" s="121"/>
+      <c r="H14" s="134"/>
       <c r="I14" s="105" t="s">
         <v>189</v>
       </c>
@@ -3388,17 +3380,17 @@
       <c r="Y14" s="76"/>
       <c r="Z14" s="32"/>
     </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="28">
       <c r="B15" s="92" t="s">
         <v>234</v>
       </c>
       <c r="C15" s="43"/>
-      <c r="D15" s="110" t="s">
+      <c r="D15" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="111"/>
-      <c r="F15" s="112"/>
-      <c r="H15" s="122"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="130"/>
+      <c r="H15" s="117"/>
       <c r="I15" s="95" t="s">
         <v>191</v>
       </c>
@@ -3438,7 +3430,7 @@
       <c r="Y15" s="76"/>
       <c r="Z15" s="32"/>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="28">
       <c r="B16" s="92" t="s">
         <v>391</v>
       </c>
@@ -3452,7 +3444,7 @@
       <c r="F16" s="45">
         <v>8</v>
       </c>
-      <c r="H16" s="120" t="s">
+      <c r="H16" s="116" t="s">
         <v>336</v>
       </c>
       <c r="I16" s="40" t="s">
@@ -3493,7 +3485,7 @@
       <c r="Y16" s="76"/>
       <c r="Z16" s="32"/>
     </row>
-    <row r="17" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" ht="28">
       <c r="B17" s="91" t="s">
         <v>14</v>
       </c>
@@ -3508,7 +3500,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="76"/>
-      <c r="H17" s="122"/>
+      <c r="H17" s="117"/>
       <c r="I17" s="40" t="s">
         <v>268</v>
       </c>
@@ -3547,7 +3539,7 @@
       <c r="Y17" s="76"/>
       <c r="Z17" s="32"/>
     </row>
-    <row r="18" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" ht="28">
       <c r="B18" s="90" t="s">
         <v>305</v>
       </c>
@@ -3562,7 +3554,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="76"/>
-      <c r="H18" s="127" t="s">
+      <c r="H18" s="118" t="s">
         <v>333</v>
       </c>
       <c r="I18" s="40" t="s">
@@ -3604,7 +3596,7 @@
       <c r="Y18" s="76"/>
       <c r="Z18" s="32"/>
     </row>
-    <row r="19" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" ht="28">
       <c r="B19" s="91" t="s">
         <v>15</v>
       </c>
@@ -3619,7 +3611,7 @@
         <v>11</v>
       </c>
       <c r="G19" s="76"/>
-      <c r="H19" s="128"/>
+      <c r="H19" s="119"/>
       <c r="I19" s="40" t="s">
         <v>270</v>
       </c>
@@ -3658,7 +3650,7 @@
       </c>
       <c r="Y19" s="76"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:26">
       <c r="B20" s="90" t="s">
         <v>306</v>
       </c>
@@ -3693,20 +3685,20 @@
       </c>
       <c r="Y20" s="76"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26">
       <c r="B21" s="92" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="8"/>
       <c r="E21" s="7"/>
       <c r="F21" s="48"/>
-      <c r="H21" s="113" t="s">
+      <c r="H21" s="125" t="s">
         <v>210</v>
       </c>
-      <c r="I21" s="114"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="114"/>
-      <c r="L21" s="115"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="126"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="127"/>
       <c r="N21" s="97" t="s">
         <v>77</v>
       </c>
@@ -3726,14 +3718,14 @@
       </c>
       <c r="Y21" s="76"/>
     </row>
-    <row r="22" spans="2:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:26" ht="42">
       <c r="B22" s="90" t="s">
         <v>307</v>
       </c>
       <c r="C22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="48"/>
-      <c r="H22" s="129" t="s">
+      <c r="H22" s="120" t="s">
         <v>335</v>
       </c>
       <c r="I22" s="95" t="s">
@@ -3768,14 +3760,14 @@
       </c>
       <c r="Y22" s="76"/>
     </row>
-    <row r="23" spans="2:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26" ht="42">
       <c r="B23" s="92" t="s">
         <v>236</v>
       </c>
       <c r="C23" s="8"/>
       <c r="E23" s="7"/>
       <c r="F23" s="48"/>
-      <c r="H23" s="130"/>
+      <c r="H23" s="121"/>
       <c r="I23" s="95" t="s">
         <v>196</v>
       </c>
@@ -3808,7 +3800,7 @@
       </c>
       <c r="Y23" s="76"/>
     </row>
-    <row r="24" spans="2:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" ht="42">
       <c r="B24" s="92" t="s">
         <v>237</v>
       </c>
@@ -3851,7 +3843,7 @@
       </c>
       <c r="Y24" s="76"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26">
       <c r="B25" s="92" t="s">
         <v>392</v>
       </c>
@@ -3878,20 +3870,20 @@
       </c>
       <c r="Y25" s="76"/>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26">
       <c r="B26" s="92" t="s">
         <v>393</v>
       </c>
       <c r="D26" s="46"/>
       <c r="E26" s="7"/>
       <c r="F26" s="48"/>
-      <c r="H26" s="113" t="s">
+      <c r="H26" s="125" t="s">
         <v>211</v>
       </c>
-      <c r="I26" s="114"/>
-      <c r="J26" s="114"/>
-      <c r="K26" s="114"/>
-      <c r="L26" s="115"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="126"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="127"/>
       <c r="N26" s="97" t="s">
         <v>387</v>
       </c>
@@ -3913,13 +3905,13 @@
       </c>
       <c r="Y26" s="76"/>
     </row>
-    <row r="27" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:26" ht="28">
       <c r="B27" s="90" t="s">
         <v>394</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="48"/>
-      <c r="H27" s="131" t="s">
+      <c r="H27" s="122" t="s">
         <v>335</v>
       </c>
       <c r="I27" s="95" t="s">
@@ -3952,14 +3944,14 @@
       </c>
       <c r="Y27" s="76"/>
     </row>
-    <row r="28" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:26" ht="28">
       <c r="B28" s="50" t="s">
         <v>395</v>
       </c>
       <c r="D28" s="71"/>
       <c r="E28" s="67"/>
       <c r="F28" s="72"/>
-      <c r="H28" s="132"/>
+      <c r="H28" s="123"/>
       <c r="I28" s="96" t="s">
         <v>348</v>
       </c>
@@ -3990,14 +3982,14 @@
       </c>
       <c r="Y28" s="76"/>
     </row>
-    <row r="29" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:26" ht="28">
       <c r="B29" s="92" t="s">
         <v>396</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="67"/>
       <c r="F29" s="72"/>
-      <c r="H29" s="132"/>
+      <c r="H29" s="123"/>
       <c r="I29" s="95" t="s">
         <v>207</v>
       </c>
@@ -4027,12 +4019,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="30" spans="2:26" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:26" s="66" customFormat="1" ht="28">
       <c r="B30" s="2"/>
       <c r="D30" s="46"/>
       <c r="E30" s="7"/>
       <c r="F30" s="48"/>
-      <c r="H30" s="132"/>
+      <c r="H30" s="123"/>
       <c r="I30" s="96" t="s">
         <v>357</v>
       </c>
@@ -4062,11 +4054,11 @@
         <v>326</v>
       </c>
     </row>
-    <row r="31" spans="2:26" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:26" s="66" customFormat="1" ht="28">
       <c r="D31" s="46"/>
       <c r="E31" s="7"/>
       <c r="F31" s="48"/>
-      <c r="H31" s="133"/>
+      <c r="H31" s="124"/>
       <c r="I31" s="96" t="s">
         <v>64</v>
       </c>
@@ -4096,11 +4088,11 @@
         <v>327</v>
       </c>
     </row>
-    <row r="32" spans="2:26" ht="60" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:26" ht="56">
       <c r="D32" s="46"/>
       <c r="E32" s="7"/>
       <c r="F32" s="48"/>
-      <c r="H32" s="123" t="s">
+      <c r="H32" s="112" t="s">
         <v>369</v>
       </c>
       <c r="I32" s="96" t="s">
@@ -4131,11 +4123,11 @@
         <v>328</v>
       </c>
     </row>
-    <row r="33" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:24" ht="28">
       <c r="D33" s="46"/>
       <c r="E33" s="7"/>
       <c r="F33" s="48"/>
-      <c r="H33" s="124"/>
+      <c r="H33" s="113"/>
       <c r="I33" s="96" t="s">
         <v>343</v>
       </c>
@@ -4163,7 +4155,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:24" ht="28">
       <c r="D34" s="46"/>
       <c r="E34" s="7"/>
       <c r="F34" s="48"/>
@@ -4198,11 +4190,11 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:24" ht="28">
       <c r="D35" s="46"/>
       <c r="E35" s="7"/>
       <c r="F35" s="48"/>
-      <c r="H35" s="125" t="s">
+      <c r="H35" s="114" t="s">
         <v>361</v>
       </c>
       <c r="I35" s="96" t="s">
@@ -4233,11 +4225,11 @@
         <v>331</v>
       </c>
     </row>
-    <row r="36" spans="4:24" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:24" ht="30" customHeight="1">
       <c r="D36" s="51"/>
       <c r="E36" s="6"/>
       <c r="F36" s="52"/>
-      <c r="H36" s="126"/>
+      <c r="H36" s="115"/>
       <c r="I36" s="96" t="s">
         <v>311</v>
       </c>
@@ -4266,7 +4258,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:24" ht="28">
       <c r="D37" s="51"/>
       <c r="E37" s="7"/>
       <c r="F37" s="52"/>
@@ -4300,7 +4292,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="38" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:24" ht="28">
       <c r="H38" s="82">
         <v>11</v>
       </c>
@@ -4332,7 +4324,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="39" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:24">
       <c r="N39" s="97" t="s">
         <v>326</v>
       </c>
@@ -4349,7 +4341,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:24">
       <c r="N40" s="97" t="s">
         <v>327</v>
       </c>
@@ -4366,7 +4358,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="41" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:24">
       <c r="N41" s="97" t="s">
         <v>328</v>
       </c>
@@ -4383,7 +4375,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:24">
       <c r="H42" s="70"/>
       <c r="I42" s="66"/>
       <c r="J42" s="66"/>
@@ -4404,7 +4396,7 @@
       <c r="W42" s="42"/>
       <c r="X42" s="25"/>
     </row>
-    <row r="43" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:24">
       <c r="N43" s="97" t="s">
         <v>330</v>
       </c>
@@ -4421,7 +4413,7 @@
       <c r="W43" s="42"/>
       <c r="X43" s="25"/>
     </row>
-    <row r="44" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:24">
       <c r="D44" s="54"/>
       <c r="E44" s="54"/>
       <c r="F44" s="54"/>
@@ -4444,7 +4436,7 @@
       <c r="W44" s="42"/>
       <c r="X44" s="25"/>
     </row>
-    <row r="45" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:24">
       <c r="D45" s="55"/>
       <c r="E45" s="56"/>
       <c r="F45" s="57"/>
@@ -4464,7 +4456,7 @@
       <c r="W45" s="42"/>
       <c r="X45" s="25"/>
     </row>
-    <row r="46" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:24">
       <c r="D46" s="55"/>
       <c r="E46" s="56"/>
       <c r="F46" s="57"/>
@@ -4484,7 +4476,7 @@
       <c r="W46" s="42"/>
       <c r="X46" s="25"/>
     </row>
-    <row r="47" spans="4:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:24" ht="32.25" customHeight="1">
       <c r="D47" s="55"/>
       <c r="E47" s="56"/>
       <c r="F47" s="57"/>
@@ -4504,7 +4496,7 @@
       <c r="W47" s="42"/>
       <c r="X47" s="25"/>
     </row>
-    <row r="48" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:24">
       <c r="D48" s="55"/>
       <c r="E48" s="58"/>
       <c r="F48" s="57"/>
@@ -4524,7 +4516,7 @@
       <c r="W48" s="42"/>
       <c r="X48" s="25"/>
     </row>
-    <row r="49" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:24">
       <c r="D49" s="55"/>
       <c r="E49" s="56"/>
       <c r="F49" s="57"/>
@@ -4544,7 +4536,7 @@
       <c r="W49" s="42"/>
       <c r="X49" s="25"/>
     </row>
-    <row r="50" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:24">
       <c r="N50" s="41" t="s">
         <v>294</v>
       </c>
@@ -4561,7 +4553,7 @@
       <c r="W50" s="42"/>
       <c r="X50" s="25"/>
     </row>
-    <row r="51" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:24">
       <c r="P51" s="25"/>
       <c r="Q51" s="25"/>
       <c r="S51" s="25"/>
@@ -4571,7 +4563,7 @@
       <c r="W51" s="25"/>
       <c r="X51" s="25"/>
     </row>
-    <row r="52" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:24">
       <c r="P52" s="25"/>
       <c r="Q52" s="25"/>
       <c r="S52" s="25"/>
@@ -4581,7 +4573,7 @@
       <c r="W52" s="25"/>
       <c r="X52" s="25"/>
     </row>
-    <row r="53" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:24">
       <c r="P53" s="25"/>
       <c r="Q53" s="25"/>
       <c r="S53" s="25"/>
@@ -4591,7 +4583,7 @@
       <c r="W53" s="25"/>
       <c r="X53" s="25"/>
     </row>
-    <row r="54" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:24">
       <c r="O54" s="25"/>
       <c r="P54" s="25"/>
       <c r="Q54" s="25"/>
@@ -4602,7 +4594,7 @@
       <c r="W54" s="25"/>
       <c r="X54" s="25"/>
     </row>
-    <row r="55" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:24">
       <c r="D55" s="59"/>
       <c r="O55" s="25"/>
       <c r="P55" s="25"/>
@@ -4614,7 +4606,7 @@
       <c r="W55" s="25"/>
       <c r="X55" s="25"/>
     </row>
-    <row r="56" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:24">
       <c r="D56" s="59"/>
       <c r="H56" s="53"/>
       <c r="O56" s="25"/>
@@ -4627,7 +4619,7 @@
       <c r="W56" s="25"/>
       <c r="X56" s="25"/>
     </row>
-    <row r="57" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:24">
       <c r="H57" s="53"/>
       <c r="O57" s="25"/>
       <c r="P57" s="25"/>
@@ -4639,7 +4631,7 @@
       <c r="W57" s="25"/>
       <c r="X57" s="25"/>
     </row>
-    <row r="58" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:24">
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
       <c r="Q58" s="25"/>
@@ -4650,7 +4642,7 @@
       <c r="W58" s="25"/>
       <c r="X58" s="25"/>
     </row>
-    <row r="59" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:24">
       <c r="D59" s="59"/>
       <c r="O59" s="25"/>
       <c r="P59" s="25"/>
@@ -4662,7 +4654,7 @@
       <c r="W59" s="25"/>
       <c r="X59" s="25"/>
     </row>
-    <row r="60" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:24">
       <c r="D60" s="59"/>
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
@@ -4674,7 +4666,7 @@
       <c r="W60" s="25"/>
       <c r="X60" s="25"/>
     </row>
-    <row r="61" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:24">
       <c r="D61" s="59"/>
       <c r="O61" s="25"/>
       <c r="P61" s="25"/>
@@ -4686,7 +4678,7 @@
       <c r="W61" s="25"/>
       <c r="X61" s="25"/>
     </row>
-    <row r="62" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:24">
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="25"/>
@@ -4697,7 +4689,7 @@
       <c r="W62" s="25"/>
       <c r="X62" s="25"/>
     </row>
-    <row r="63" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:24">
       <c r="O63" s="25"/>
       <c r="P63" s="25"/>
       <c r="Q63" s="25"/>
@@ -4708,7 +4700,7 @@
       <c r="W63" s="25"/>
       <c r="X63" s="25"/>
     </row>
-    <row r="64" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:24">
       <c r="O64" s="25"/>
       <c r="P64" s="25"/>
       <c r="Q64" s="25"/>
@@ -4719,7 +4711,7 @@
       <c r="W64" s="25"/>
       <c r="X64" s="25"/>
     </row>
-    <row r="65" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:22">
       <c r="O65" s="25"/>
       <c r="P65" s="25"/>
       <c r="Q65" s="25"/>
@@ -4728,43 +4720,48 @@
       <c r="U65" s="25"/>
       <c r="V65" s="25"/>
     </row>
-    <row r="66" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:22">
       <c r="P66" s="25"/>
       <c r="U66" s="25"/>
       <c r="V66" s="25"/>
     </row>
-    <row r="67" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:22">
       <c r="P67" s="25"/>
       <c r="U67" s="25"/>
       <c r="V67" s="25"/>
     </row>
-    <row r="72" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:22">
       <c r="D72" s="60"/>
       <c r="E72" s="60"/>
       <c r="F72" s="60"/>
     </row>
-    <row r="73" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:22">
       <c r="D73" s="61"/>
       <c r="E73" s="62"/>
       <c r="F73" s="63"/>
     </row>
-    <row r="74" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:22">
       <c r="D74" s="61"/>
       <c r="E74" s="62"/>
       <c r="F74" s="63"/>
     </row>
-    <row r="75" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:22">
       <c r="D75" s="61"/>
       <c r="E75" s="62"/>
       <c r="F75" s="63"/>
     </row>
-    <row r="76" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:22">
       <c r="D76" s="61"/>
       <c r="E76" s="62"/>
       <c r="F76" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="H32:H33"/>
@@ -4777,19 +4774,19 @@
     <mergeCell ref="H26:L26"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
     <mergeCell ref="H12:H15"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <ignoredErrors>
     <ignoredError sqref="H9" numberStoredAsText="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4799,7 +4796,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -4807,7 +4804,7 @@
     <col min="4" max="4" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>173</v>
       </c>
@@ -4821,7 +4818,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="65" customFormat="1">
       <c r="A2" s="75">
         <v>42296</v>
       </c>
@@ -4831,31 +4828,31 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="65" customFormat="1">
       <c r="A3" s="75"/>
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
       <c r="D3" s="73"/>
     </row>
-    <row r="4" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="65" customFormat="1">
       <c r="A4" s="75"/>
       <c r="B4" s="107"/>
       <c r="C4" s="107"/>
       <c r="D4" s="73"/>
     </row>
-    <row r="5" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="65" customFormat="1">
       <c r="A5" s="75"/>
       <c r="B5" s="107"/>
       <c r="C5" s="107"/>
       <c r="D5" s="73"/>
     </row>
-    <row r="6" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="65" customFormat="1">
       <c r="A6" s="108"/>
       <c r="B6" s="109"/>
       <c r="C6" s="109"/>
       <c r="D6" s="109"/>
     </row>
-    <row r="7" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="65" customFormat="1">
       <c r="A7" s="75">
         <v>42293</v>
       </c>
@@ -4865,7 +4862,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="65" customFormat="1">
       <c r="A8" s="75"/>
       <c r="B8" s="107"/>
       <c r="C8" s="107"/>
@@ -4873,7 +4870,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="65" customFormat="1">
       <c r="A9" s="75"/>
       <c r="B9" s="107"/>
       <c r="C9" s="107"/>
@@ -4881,7 +4878,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="65" customFormat="1">
       <c r="A10" s="75"/>
       <c r="B10" s="107"/>
       <c r="C10" s="107"/>
@@ -4889,13 +4886,13 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="65" customFormat="1">
       <c r="A11" s="108"/>
       <c r="B11" s="109"/>
       <c r="C11" s="109"/>
       <c r="D11" s="109"/>
     </row>
-    <row r="12" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="65" customFormat="1">
       <c r="A12" s="75">
         <v>42223</v>
       </c>
@@ -4907,7 +4904,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="65" customFormat="1">
       <c r="A13" s="75"/>
       <c r="B13" s="107"/>
       <c r="C13" s="107"/>
@@ -4915,13 +4912,13 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="65" customFormat="1">
       <c r="A14" s="108"/>
       <c r="B14" s="109"/>
       <c r="C14" s="109"/>
       <c r="D14" s="109"/>
     </row>
-    <row r="15" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="65" customFormat="1">
       <c r="A15" s="75">
         <v>42179</v>
       </c>
@@ -4933,7 +4930,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="65" customFormat="1">
       <c r="A16" s="75"/>
       <c r="B16" s="107"/>
       <c r="C16" s="107"/>
@@ -4941,7 +4938,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="65" customFormat="1">
       <c r="A17" s="75"/>
       <c r="B17" s="107"/>
       <c r="C17" s="107"/>
@@ -4949,7 +4946,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="65" customFormat="1">
       <c r="A18" s="75"/>
       <c r="B18" s="107"/>
       <c r="C18" s="107"/>
@@ -4957,7 +4954,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" s="65" customFormat="1">
       <c r="A19" s="75"/>
       <c r="B19" s="107"/>
       <c r="C19" s="107"/>
@@ -4965,7 +4962,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="65" customFormat="1">
       <c r="A20" s="75"/>
       <c r="B20" s="107"/>
       <c r="C20" s="107"/>
@@ -4973,7 +4970,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="65" customFormat="1">
       <c r="A21" s="75"/>
       <c r="B21" s="107"/>
       <c r="C21" s="107"/>
@@ -4981,7 +4978,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" s="65" customFormat="1">
       <c r="A22" s="75"/>
       <c r="B22" s="107"/>
       <c r="C22" s="107"/>
@@ -4989,7 +4986,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="65" customFormat="1">
       <c r="A23" s="75"/>
       <c r="B23" s="107"/>
       <c r="C23" s="107"/>
@@ -4997,7 +4994,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="65" customFormat="1">
       <c r="A24" s="75"/>
       <c r="B24" s="107"/>
       <c r="C24" s="107"/>
@@ -5005,7 +5002,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="65" customFormat="1">
       <c r="A25" s="75"/>
       <c r="B25" s="107"/>
       <c r="C25" s="107"/>
@@ -5013,13 +5010,13 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" s="65" customFormat="1">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="74" customFormat="1">
       <c r="A27" s="75">
         <v>42165</v>
       </c>
@@ -5033,91 +5030,91 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" s="74" customFormat="1">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" s="78" customFormat="1">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="74" customFormat="1">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="74" customFormat="1">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" s="74" customFormat="1">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" s="74" customFormat="1">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" s="74" customFormat="1">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" s="74" customFormat="1">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" s="74" customFormat="1">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" s="74" customFormat="1">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" s="78" customFormat="1">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" s="76" customFormat="1">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" s="78" customFormat="1">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" s="74" customFormat="1">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" s="65" customFormat="1">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -5126,7 +5123,12 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5136,707 +5138,707 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="105.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="101" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" s="102" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1">
       <c r="A90" s="103" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1">
       <c r="A97" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" s="103" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" s="93" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="93" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="93" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="103" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="103" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="103" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" s="93" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="93" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="93" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" s="103" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" s="103" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" s="103" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141" s="93" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1">
       <c r="A143" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1">
       <c r="A145" s="93" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1">
       <c r="A146" s="93" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1">
       <c r="A147" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1">
       <c r="A149" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1">
       <c r="A150" s="103" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1">
       <c r="A151" s="103" t="s">
         <v>354</v>
       </c>
@@ -5844,7 +5846,12 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5854,14 +5861,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>212</v>
       </c>
@@ -5872,7 +5879,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -5883,7 +5890,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -5894,7 +5901,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -5905,7 +5912,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -5916,7 +5923,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="65" customFormat="1">
       <c r="A6" s="65" t="s">
         <v>241</v>
       </c>
@@ -5927,7 +5934,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -5938,7 +5945,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -5949,7 +5956,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -5960,7 +5967,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>219</v>
       </c>
@@ -5971,7 +5978,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>220</v>
       </c>
@@ -5982,7 +5989,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="65" t="s">
         <v>239</v>
       </c>
@@ -5995,5 +6002,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BOM fully parsed. Initial verification in place. Needs OS verification and verification that all system and adapter columns aren't empty.
</commit_message>
<xml_diff>
--- a/15C-Red-BOM-2015-10-19.xlsx
+++ b/15C-Red-BOM-2015-10-19.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26408"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbothwell/Documents/Git/jar-verify/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-34460" yWindow="560" windowWidth="29500" windowHeight="20380"/>
   </bookViews>
@@ -1723,7 +1718,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="170">
+  <cellStyleXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1894,8 +1889,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2187,24 +2188,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2245,6 +2228,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2257,8 +2249,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="170">
+  <cellStyles count="176">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2343,6 +2347,9 @@
     <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2427,6 +2434,9 @@
     <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -2729,11 +2739,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="2"/>
     <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
@@ -2762,54 +2772,54 @@
     <col min="25" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+    <row r="1" spans="1:26" ht="18">
+      <c r="A1" s="135" t="s">
         <v>403</v>
       </c>
-      <c r="B1" s="117"/>
+      <c r="B1" s="111"/>
       <c r="C1" s="110"/>
       <c r="D1" s="110"/>
     </row>
-    <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="117" t="s">
+    <row r="2" spans="1:26" ht="18">
+      <c r="A2" s="111" t="s">
         <v>404</v>
       </c>
-      <c r="B2" s="117"/>
-    </row>
-    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="111"/>
+    </row>
+    <row r="4" spans="1:26" ht="15">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="111" t="s">
+      <c r="D4" s="132" t="s">
         <v>407</v>
       </c>
-      <c r="E4" s="112"/>
-      <c r="F4" s="113"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="134"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="111" t="s">
+      <c r="H4" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="113"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="134"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="111" t="s">
+      <c r="N4" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="O4" s="133"/>
+      <c r="P4" s="133"/>
+      <c r="Q4" s="133"/>
+      <c r="R4" s="133"/>
+      <c r="S4" s="133"/>
+      <c r="T4" s="133"/>
+      <c r="U4" s="133"/>
+      <c r="V4" s="133"/>
+      <c r="W4" s="133"/>
+      <c r="X4" s="134"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="B5" s="88" t="s">
         <v>51</v>
       </c>
@@ -2874,24 +2884,24 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="B6" s="89" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="115"/>
-      <c r="F6" s="116"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="114" t="s">
+      <c r="H6" s="125" t="s">
         <v>208</v>
       </c>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="116"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
       <c r="M6" s="24"/>
       <c r="N6" s="97" t="s">
         <v>9</v>
@@ -2929,7 +2939,7 @@
       <c r="Y6" s="76"/>
       <c r="Z6" s="25"/>
     </row>
-    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="28">
       <c r="B7" s="90" t="s">
         <v>238</v>
       </c>
@@ -2996,7 +3006,7 @@
       <c r="Y7" s="76"/>
       <c r="Z7" s="32"/>
     </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="28">
       <c r="B8" s="90" t="s">
         <v>302</v>
       </c>
@@ -3060,7 +3070,7 @@
       <c r="Y8" s="76"/>
       <c r="Z8" s="32"/>
     </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="28">
       <c r="B9" s="92" t="s">
         <v>232</v>
       </c>
@@ -3124,7 +3134,7 @@
       <c r="Y9" s="76"/>
       <c r="Z9" s="32"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="B10" s="90" t="s">
         <v>303</v>
       </c>
@@ -3171,7 +3181,7 @@
       <c r="Y10" s="76"/>
       <c r="Z10" s="32"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="B11" s="92" t="s">
         <v>231</v>
       </c>
@@ -3186,13 +3196,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="114" t="s">
+      <c r="H11" s="125" t="s">
         <v>209</v>
       </c>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="116"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="127"/>
       <c r="N11" s="64" t="s">
         <v>285</v>
       </c>
@@ -3225,7 +3235,7 @@
       <c r="Y11" s="76"/>
       <c r="Z11" s="32"/>
     </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="28">
       <c r="B12" s="90" t="s">
         <v>304</v>
       </c>
@@ -3240,7 +3250,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="122" t="s">
+      <c r="H12" s="116" t="s">
         <v>335</v>
       </c>
       <c r="I12" s="95" t="s">
@@ -3284,7 +3294,7 @@
       <c r="Y12" s="76"/>
       <c r="Z12" s="32"/>
     </row>
-    <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="28">
       <c r="B13" s="90" t="s">
         <v>233</v>
       </c>
@@ -3299,7 +3309,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="H13" s="134"/>
+      <c r="H13" s="131"/>
       <c r="I13" s="95" t="s">
         <v>185</v>
       </c>
@@ -3341,12 +3351,12 @@
       <c r="Y13" s="76"/>
       <c r="Z13" s="32"/>
     </row>
-    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="28">
       <c r="B14" s="90" t="s">
         <v>390</v>
       </c>
       <c r="C14" s="43"/>
-      <c r="H14" s="134"/>
+      <c r="H14" s="131"/>
       <c r="I14" s="105" t="s">
         <v>189</v>
       </c>
@@ -3389,17 +3399,17 @@
       <c r="Y14" s="76"/>
       <c r="Z14" s="32"/>
     </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="28">
       <c r="B15" s="92" t="s">
         <v>234</v>
       </c>
       <c r="C15" s="43"/>
-      <c r="D15" s="131" t="s">
+      <c r="D15" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="132"/>
-      <c r="F15" s="133"/>
-      <c r="H15" s="123"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="130"/>
+      <c r="H15" s="117"/>
       <c r="I15" s="95" t="s">
         <v>191</v>
       </c>
@@ -3439,7 +3449,7 @@
       <c r="Y15" s="76"/>
       <c r="Z15" s="32"/>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="28">
       <c r="B16" s="92" t="s">
         <v>391</v>
       </c>
@@ -3453,7 +3463,7 @@
       <c r="F16" s="45">
         <v>8</v>
       </c>
-      <c r="H16" s="122" t="s">
+      <c r="H16" s="116" t="s">
         <v>336</v>
       </c>
       <c r="I16" s="40" t="s">
@@ -3494,7 +3504,7 @@
       <c r="Y16" s="76"/>
       <c r="Z16" s="32"/>
     </row>
-    <row r="17" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" ht="28">
       <c r="B17" s="91" t="s">
         <v>14</v>
       </c>
@@ -3509,7 +3519,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="76"/>
-      <c r="H17" s="123"/>
+      <c r="H17" s="117"/>
       <c r="I17" s="40" t="s">
         <v>268</v>
       </c>
@@ -3548,7 +3558,7 @@
       <c r="Y17" s="76"/>
       <c r="Z17" s="32"/>
     </row>
-    <row r="18" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" ht="28">
       <c r="B18" s="90" t="s">
         <v>305</v>
       </c>
@@ -3563,7 +3573,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="76"/>
-      <c r="H18" s="124" t="s">
+      <c r="H18" s="118" t="s">
         <v>333</v>
       </c>
       <c r="I18" s="40" t="s">
@@ -3605,7 +3615,7 @@
       <c r="Y18" s="76"/>
       <c r="Z18" s="32"/>
     </row>
-    <row r="19" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" ht="28">
       <c r="B19" s="91" t="s">
         <v>15</v>
       </c>
@@ -3620,7 +3630,7 @@
         <v>11</v>
       </c>
       <c r="G19" s="76"/>
-      <c r="H19" s="125"/>
+      <c r="H19" s="119"/>
       <c r="I19" s="40" t="s">
         <v>270</v>
       </c>
@@ -3659,7 +3669,7 @@
       </c>
       <c r="Y19" s="76"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:26">
       <c r="B20" s="90" t="s">
         <v>306</v>
       </c>
@@ -3694,20 +3704,20 @@
       </c>
       <c r="Y20" s="76"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26">
       <c r="B21" s="92" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="8"/>
       <c r="E21" s="7"/>
       <c r="F21" s="48"/>
-      <c r="H21" s="114" t="s">
+      <c r="H21" s="125" t="s">
         <v>210</v>
       </c>
-      <c r="I21" s="115"/>
-      <c r="J21" s="115"/>
-      <c r="K21" s="115"/>
-      <c r="L21" s="116"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="126"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="127"/>
       <c r="N21" s="97" t="s">
         <v>77</v>
       </c>
@@ -3727,14 +3737,14 @@
       </c>
       <c r="Y21" s="76"/>
     </row>
-    <row r="22" spans="2:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:26" ht="42">
       <c r="B22" s="90" t="s">
         <v>307</v>
       </c>
       <c r="C22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="48"/>
-      <c r="H22" s="126" t="s">
+      <c r="H22" s="120" t="s">
         <v>335</v>
       </c>
       <c r="I22" s="95" t="s">
@@ -3769,14 +3779,15 @@
       </c>
       <c r="Y22" s="76"/>
     </row>
-    <row r="23" spans="2:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26" ht="42">
       <c r="B23" s="92" t="s">
         <v>236</v>
       </c>
       <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="7"/>
       <c r="F23" s="48"/>
-      <c r="H23" s="127"/>
+      <c r="H23" s="121"/>
       <c r="I23" s="95" t="s">
         <v>196</v>
       </c>
@@ -3809,7 +3820,7 @@
       </c>
       <c r="Y23" s="76"/>
     </row>
-    <row r="24" spans="2:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" ht="42">
       <c r="B24" s="92" t="s">
         <v>237</v>
       </c>
@@ -3852,7 +3863,7 @@
       </c>
       <c r="Y24" s="76"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26">
       <c r="B25" s="92" t="s">
         <v>392</v>
       </c>
@@ -3879,20 +3890,20 @@
       </c>
       <c r="Y25" s="76"/>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26">
       <c r="B26" s="92" t="s">
         <v>393</v>
       </c>
       <c r="D26" s="46"/>
       <c r="E26" s="7"/>
       <c r="F26" s="48"/>
-      <c r="H26" s="114" t="s">
+      <c r="H26" s="125" t="s">
         <v>211</v>
       </c>
-      <c r="I26" s="115"/>
-      <c r="J26" s="115"/>
-      <c r="K26" s="115"/>
-      <c r="L26" s="116"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="126"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="127"/>
       <c r="N26" s="97" t="s">
         <v>387</v>
       </c>
@@ -3914,13 +3925,13 @@
       </c>
       <c r="Y26" s="76"/>
     </row>
-    <row r="27" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:26" ht="28">
       <c r="B27" s="90" t="s">
         <v>394</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="48"/>
-      <c r="H27" s="128" t="s">
+      <c r="H27" s="122" t="s">
         <v>335</v>
       </c>
       <c r="I27" s="95" t="s">
@@ -3953,14 +3964,14 @@
       </c>
       <c r="Y27" s="76"/>
     </row>
-    <row r="28" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:26" ht="28">
       <c r="B28" s="50" t="s">
         <v>395</v>
       </c>
       <c r="D28" s="71"/>
       <c r="E28" s="67"/>
       <c r="F28" s="72"/>
-      <c r="H28" s="129"/>
+      <c r="H28" s="123"/>
       <c r="I28" s="96" t="s">
         <v>348</v>
       </c>
@@ -3991,14 +4002,14 @@
       </c>
       <c r="Y28" s="76"/>
     </row>
-    <row r="29" spans="2:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:26" ht="28">
       <c r="B29" s="92" t="s">
         <v>396</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="67"/>
       <c r="F29" s="72"/>
-      <c r="H29" s="129"/>
+      <c r="H29" s="123"/>
       <c r="I29" s="95" t="s">
         <v>207</v>
       </c>
@@ -4028,12 +4039,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="30" spans="2:26" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:26" s="66" customFormat="1" ht="28">
       <c r="B30" s="2"/>
       <c r="D30" s="46"/>
       <c r="E30" s="7"/>
       <c r="F30" s="48"/>
-      <c r="H30" s="129"/>
+      <c r="H30" s="123"/>
       <c r="I30" s="96" t="s">
         <v>357</v>
       </c>
@@ -4063,11 +4074,11 @@
         <v>326</v>
       </c>
     </row>
-    <row r="31" spans="2:26" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:26" s="66" customFormat="1" ht="28">
       <c r="D31" s="46"/>
       <c r="E31" s="7"/>
       <c r="F31" s="48"/>
-      <c r="H31" s="130"/>
+      <c r="H31" s="124"/>
       <c r="I31" s="96" t="s">
         <v>64</v>
       </c>
@@ -4097,11 +4108,11 @@
         <v>327</v>
       </c>
     </row>
-    <row r="32" spans="2:26" ht="60" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:26" ht="56">
       <c r="D32" s="46"/>
       <c r="E32" s="7"/>
       <c r="F32" s="48"/>
-      <c r="H32" s="118" t="s">
+      <c r="H32" s="112" t="s">
         <v>369</v>
       </c>
       <c r="I32" s="96" t="s">
@@ -4132,11 +4143,11 @@
         <v>328</v>
       </c>
     </row>
-    <row r="33" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:24" ht="28">
       <c r="D33" s="46"/>
       <c r="E33" s="7"/>
       <c r="F33" s="48"/>
-      <c r="H33" s="119"/>
+      <c r="H33" s="113"/>
       <c r="I33" s="96" t="s">
         <v>343</v>
       </c>
@@ -4164,7 +4175,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:24" ht="28">
       <c r="D34" s="46"/>
       <c r="E34" s="7"/>
       <c r="F34" s="48"/>
@@ -4199,11 +4210,11 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:24" ht="28">
       <c r="D35" s="46"/>
       <c r="E35" s="7"/>
       <c r="F35" s="48"/>
-      <c r="H35" s="120" t="s">
+      <c r="H35" s="114" t="s">
         <v>361</v>
       </c>
       <c r="I35" s="96" t="s">
@@ -4234,11 +4245,11 @@
         <v>331</v>
       </c>
     </row>
-    <row r="36" spans="4:24" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:24" ht="30" customHeight="1">
       <c r="D36" s="51"/>
       <c r="E36" s="6"/>
       <c r="F36" s="52"/>
-      <c r="H36" s="121"/>
+      <c r="H36" s="115"/>
       <c r="I36" s="96" t="s">
         <v>311</v>
       </c>
@@ -4267,7 +4278,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:24" ht="28">
       <c r="D37" s="51"/>
       <c r="E37" s="7"/>
       <c r="F37" s="52"/>
@@ -4301,7 +4312,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="38" spans="4:24" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:24" ht="28">
       <c r="H38" s="82">
         <v>11</v>
       </c>
@@ -4333,7 +4344,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="39" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:24">
       <c r="N39" s="97" t="s">
         <v>326</v>
       </c>
@@ -4350,7 +4361,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:24">
       <c r="N40" s="97" t="s">
         <v>327</v>
       </c>
@@ -4367,7 +4378,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="41" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:24">
       <c r="N41" s="97" t="s">
         <v>328</v>
       </c>
@@ -4384,7 +4395,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:24">
       <c r="H42" s="70"/>
       <c r="I42" s="66"/>
       <c r="J42" s="66"/>
@@ -4405,7 +4416,7 @@
       <c r="W42" s="42"/>
       <c r="X42" s="25"/>
     </row>
-    <row r="43" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:24">
       <c r="N43" s="97" t="s">
         <v>330</v>
       </c>
@@ -4422,7 +4433,7 @@
       <c r="W43" s="42"/>
       <c r="X43" s="25"/>
     </row>
-    <row r="44" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:24">
       <c r="D44" s="54"/>
       <c r="E44" s="54"/>
       <c r="F44" s="54"/>
@@ -4445,7 +4456,7 @@
       <c r="W44" s="42"/>
       <c r="X44" s="25"/>
     </row>
-    <row r="45" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:24">
       <c r="D45" s="55"/>
       <c r="E45" s="56"/>
       <c r="F45" s="57"/>
@@ -4465,7 +4476,7 @@
       <c r="W45" s="42"/>
       <c r="X45" s="25"/>
     </row>
-    <row r="46" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:24">
       <c r="D46" s="55"/>
       <c r="E46" s="56"/>
       <c r="F46" s="57"/>
@@ -4485,7 +4496,7 @@
       <c r="W46" s="42"/>
       <c r="X46" s="25"/>
     </row>
-    <row r="47" spans="4:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:24" ht="32.25" customHeight="1">
       <c r="D47" s="55"/>
       <c r="E47" s="56"/>
       <c r="F47" s="57"/>
@@ -4505,7 +4516,7 @@
       <c r="W47" s="42"/>
       <c r="X47" s="25"/>
     </row>
-    <row r="48" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:24">
       <c r="D48" s="55"/>
       <c r="E48" s="58"/>
       <c r="F48" s="57"/>
@@ -4525,7 +4536,7 @@
       <c r="W48" s="42"/>
       <c r="X48" s="25"/>
     </row>
-    <row r="49" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:24">
       <c r="D49" s="55"/>
       <c r="E49" s="56"/>
       <c r="F49" s="57"/>
@@ -4545,7 +4556,7 @@
       <c r="W49" s="42"/>
       <c r="X49" s="25"/>
     </row>
-    <row r="50" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:24">
       <c r="N50" s="41" t="s">
         <v>294</v>
       </c>
@@ -4562,7 +4573,7 @@
       <c r="W50" s="42"/>
       <c r="X50" s="25"/>
     </row>
-    <row r="51" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:24">
       <c r="P51" s="25"/>
       <c r="Q51" s="25"/>
       <c r="S51" s="25"/>
@@ -4572,7 +4583,7 @@
       <c r="W51" s="25"/>
       <c r="X51" s="25"/>
     </row>
-    <row r="52" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:24">
       <c r="P52" s="25"/>
       <c r="Q52" s="25"/>
       <c r="S52" s="25"/>
@@ -4582,7 +4593,7 @@
       <c r="W52" s="25"/>
       <c r="X52" s="25"/>
     </row>
-    <row r="53" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:24">
       <c r="P53" s="25"/>
       <c r="Q53" s="25"/>
       <c r="S53" s="25"/>
@@ -4592,7 +4603,7 @@
       <c r="W53" s="25"/>
       <c r="X53" s="25"/>
     </row>
-    <row r="54" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:24">
       <c r="O54" s="25"/>
       <c r="P54" s="25"/>
       <c r="Q54" s="25"/>
@@ -4603,7 +4614,7 @@
       <c r="W54" s="25"/>
       <c r="X54" s="25"/>
     </row>
-    <row r="55" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:24">
       <c r="D55" s="59"/>
       <c r="O55" s="25"/>
       <c r="P55" s="25"/>
@@ -4615,7 +4626,7 @@
       <c r="W55" s="25"/>
       <c r="X55" s="25"/>
     </row>
-    <row r="56" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:24">
       <c r="D56" s="59"/>
       <c r="H56" s="53"/>
       <c r="O56" s="25"/>
@@ -4628,7 +4639,7 @@
       <c r="W56" s="25"/>
       <c r="X56" s="25"/>
     </row>
-    <row r="57" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:24">
       <c r="H57" s="53"/>
       <c r="O57" s="25"/>
       <c r="P57" s="25"/>
@@ -4640,7 +4651,7 @@
       <c r="W57" s="25"/>
       <c r="X57" s="25"/>
     </row>
-    <row r="58" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:24">
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
       <c r="Q58" s="25"/>
@@ -4651,7 +4662,7 @@
       <c r="W58" s="25"/>
       <c r="X58" s="25"/>
     </row>
-    <row r="59" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:24">
       <c r="D59" s="59"/>
       <c r="O59" s="25"/>
       <c r="P59" s="25"/>
@@ -4663,7 +4674,7 @@
       <c r="W59" s="25"/>
       <c r="X59" s="25"/>
     </row>
-    <row r="60" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:24">
       <c r="D60" s="59"/>
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
@@ -4675,7 +4686,7 @@
       <c r="W60" s="25"/>
       <c r="X60" s="25"/>
     </row>
-    <row r="61" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:24">
       <c r="D61" s="59"/>
       <c r="O61" s="25"/>
       <c r="P61" s="25"/>
@@ -4687,7 +4698,7 @@
       <c r="W61" s="25"/>
       <c r="X61" s="25"/>
     </row>
-    <row r="62" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:24">
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="25"/>
@@ -4698,7 +4709,7 @@
       <c r="W62" s="25"/>
       <c r="X62" s="25"/>
     </row>
-    <row r="63" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:24">
       <c r="O63" s="25"/>
       <c r="P63" s="25"/>
       <c r="Q63" s="25"/>
@@ -4709,7 +4720,7 @@
       <c r="W63" s="25"/>
       <c r="X63" s="25"/>
     </row>
-    <row r="64" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:24">
       <c r="O64" s="25"/>
       <c r="P64" s="25"/>
       <c r="Q64" s="25"/>
@@ -4720,7 +4731,7 @@
       <c r="W64" s="25"/>
       <c r="X64" s="25"/>
     </row>
-    <row r="65" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:22">
       <c r="O65" s="25"/>
       <c r="P65" s="25"/>
       <c r="Q65" s="25"/>
@@ -4729,43 +4740,48 @@
       <c r="U65" s="25"/>
       <c r="V65" s="25"/>
     </row>
-    <row r="66" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:22">
       <c r="P66" s="25"/>
       <c r="U66" s="25"/>
       <c r="V66" s="25"/>
     </row>
-    <row r="67" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:22">
       <c r="P67" s="25"/>
       <c r="U67" s="25"/>
       <c r="V67" s="25"/>
     </row>
-    <row r="72" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:22">
       <c r="D72" s="60"/>
       <c r="E72" s="60"/>
       <c r="F72" s="60"/>
     </row>
-    <row r="73" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:22">
       <c r="D73" s="61"/>
       <c r="E73" s="62"/>
       <c r="F73" s="63"/>
     </row>
-    <row r="74" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:22">
       <c r="D74" s="61"/>
       <c r="E74" s="62"/>
       <c r="F74" s="63"/>
     </row>
-    <row r="75" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:22">
       <c r="D75" s="61"/>
       <c r="E75" s="62"/>
       <c r="F75" s="63"/>
     </row>
-    <row r="76" spans="4:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:22">
       <c r="D76" s="61"/>
       <c r="E76" s="62"/>
       <c r="F76" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="H32:H33"/>
@@ -4779,11 +4795,6 @@
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="H12:H15"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4791,6 +4802,11 @@
   <ignoredErrors>
     <ignoredError sqref="H9" numberStoredAsText="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4800,7 +4816,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -4808,7 +4824,7 @@
     <col min="4" max="4" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>173</v>
       </c>
@@ -4822,7 +4838,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="65" customFormat="1">
       <c r="A2" s="75">
         <v>42296</v>
       </c>
@@ -4832,31 +4848,31 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="65" customFormat="1">
       <c r="A3" s="75"/>
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
       <c r="D3" s="73"/>
     </row>
-    <row r="4" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="65" customFormat="1">
       <c r="A4" s="75"/>
       <c r="B4" s="107"/>
       <c r="C4" s="107"/>
       <c r="D4" s="73"/>
     </row>
-    <row r="5" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="65" customFormat="1">
       <c r="A5" s="75"/>
       <c r="B5" s="107"/>
       <c r="C5" s="107"/>
       <c r="D5" s="73"/>
     </row>
-    <row r="6" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="65" customFormat="1">
       <c r="A6" s="108"/>
       <c r="B6" s="109"/>
       <c r="C6" s="109"/>
       <c r="D6" s="109"/>
     </row>
-    <row r="7" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="65" customFormat="1">
       <c r="A7" s="75">
         <v>42293</v>
       </c>
@@ -4866,7 +4882,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="65" customFormat="1">
       <c r="A8" s="75"/>
       <c r="B8" s="107"/>
       <c r="C8" s="107"/>
@@ -4874,7 +4890,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="65" customFormat="1">
       <c r="A9" s="75"/>
       <c r="B9" s="107"/>
       <c r="C9" s="107"/>
@@ -4882,7 +4898,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="65" customFormat="1">
       <c r="A10" s="75"/>
       <c r="B10" s="107"/>
       <c r="C10" s="107"/>
@@ -4890,13 +4906,13 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="65" customFormat="1">
       <c r="A11" s="108"/>
       <c r="B11" s="109"/>
       <c r="C11" s="109"/>
       <c r="D11" s="109"/>
     </row>
-    <row r="12" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="65" customFormat="1">
       <c r="A12" s="75">
         <v>42223</v>
       </c>
@@ -4908,7 +4924,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="65" customFormat="1">
       <c r="A13" s="75"/>
       <c r="B13" s="107"/>
       <c r="C13" s="107"/>
@@ -4916,13 +4932,13 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="65" customFormat="1">
       <c r="A14" s="108"/>
       <c r="B14" s="109"/>
       <c r="C14" s="109"/>
       <c r="D14" s="109"/>
     </row>
-    <row r="15" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="65" customFormat="1">
       <c r="A15" s="75">
         <v>42179</v>
       </c>
@@ -4934,7 +4950,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="65" customFormat="1">
       <c r="A16" s="75"/>
       <c r="B16" s="107"/>
       <c r="C16" s="107"/>
@@ -4942,7 +4958,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="65" customFormat="1">
       <c r="A17" s="75"/>
       <c r="B17" s="107"/>
       <c r="C17" s="107"/>
@@ -4950,7 +4966,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="65" customFormat="1">
       <c r="A18" s="75"/>
       <c r="B18" s="107"/>
       <c r="C18" s="107"/>
@@ -4958,7 +4974,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" s="65" customFormat="1">
       <c r="A19" s="75"/>
       <c r="B19" s="107"/>
       <c r="C19" s="107"/>
@@ -4966,7 +4982,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="65" customFormat="1">
       <c r="A20" s="75"/>
       <c r="B20" s="107"/>
       <c r="C20" s="107"/>
@@ -4974,7 +4990,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="65" customFormat="1">
       <c r="A21" s="75"/>
       <c r="B21" s="107"/>
       <c r="C21" s="107"/>
@@ -4982,7 +4998,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" s="65" customFormat="1">
       <c r="A22" s="75"/>
       <c r="B22" s="107"/>
       <c r="C22" s="107"/>
@@ -4990,7 +5006,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="65" customFormat="1">
       <c r="A23" s="75"/>
       <c r="B23" s="107"/>
       <c r="C23" s="107"/>
@@ -4998,7 +5014,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="65" customFormat="1">
       <c r="A24" s="75"/>
       <c r="B24" s="107"/>
       <c r="C24" s="107"/>
@@ -5006,7 +5022,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="65" customFormat="1">
       <c r="A25" s="75"/>
       <c r="B25" s="107"/>
       <c r="C25" s="107"/>
@@ -5014,13 +5030,13 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" s="65" customFormat="1">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="74" customFormat="1">
       <c r="A27" s="75">
         <v>42165</v>
       </c>
@@ -5034,91 +5050,91 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" s="74" customFormat="1">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" s="78" customFormat="1">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="74" customFormat="1">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="74" customFormat="1">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" s="74" customFormat="1">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" s="74" customFormat="1">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" s="74" customFormat="1">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" s="74" customFormat="1">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" s="74" customFormat="1">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" s="74" customFormat="1">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" s="78" customFormat="1">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" s="76" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" s="76" customFormat="1">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" s="78" customFormat="1">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" s="74" customFormat="1">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" s="65" customFormat="1">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -5128,6 +5144,11 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5135,709 +5156,711 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A151"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="105.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="101" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" s="102" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1">
       <c r="A90" s="103" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1">
       <c r="A97" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" s="103" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" s="93" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="93" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="93" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="103" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="103" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="103" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" s="93" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="93" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="93" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" s="103" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" s="103" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" s="103" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141" s="93" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1">
       <c r="A143" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1">
       <c r="A145" s="93" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1">
       <c r="A146" s="93" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1">
       <c r="A147" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1">
       <c r="A149" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1">
       <c r="A150" s="103" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1">
       <c r="A151" s="103" t="s">
         <v>354</v>
       </c>
@@ -5846,6 +5869,11 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5855,14 +5883,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>212</v>
       </c>
@@ -5873,7 +5901,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -5884,7 +5912,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -5895,7 +5923,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -5906,7 +5934,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -5917,7 +5945,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="65" customFormat="1">
       <c r="A6" s="65" t="s">
         <v>241</v>
       </c>
@@ -5928,7 +5956,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -5939,7 +5967,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -5950,7 +5978,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -5961,7 +5989,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>219</v>
       </c>
@@ -5972,7 +6000,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>220</v>
       </c>
@@ -5983,7 +6011,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="65" t="s">
         <v>239</v>
       </c>
@@ -5996,5 +6024,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>